<commit_message>
Heatmap commit 1 (Glutamate done)
</commit_message>
<xml_diff>
--- a/data/082023_Mapping_unique.xlsx
+++ b/data/082023_Mapping_unique.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olegtutanov/Documents/Programming/Olink/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5168D823-E399-274D-8BF2-0141AA3E524C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A3CF91-1616-9C43-B855-03F1D1D61FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4480" yWindow="3180" windowWidth="25640" windowHeight="14440" xr2:uid="{2D7CE3BD-EF66-D84A-A92E-36ED3E223C28}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="136">
   <si>
     <t>SampleID</t>
   </si>
@@ -125,9 +125,6 @@
     <t>BAD1</t>
   </si>
   <si>
-    <t>Bakeoff DiFi</t>
-  </si>
-  <si>
     <t>BAD2</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>BAC1</t>
   </si>
   <si>
-    <t>Bakeoff CC-CR</t>
-  </si>
-  <si>
     <t>BAC2</t>
   </si>
   <si>
@@ -203,31 +197,13 @@
     <t>Untreated</t>
   </si>
   <si>
-    <t>DiFi Supermere Day 0</t>
-  </si>
-  <si>
-    <t>DiFi Supermere Day 4</t>
-  </si>
-  <si>
-    <t>DiFi Supermere Day 2</t>
-  </si>
-  <si>
-    <t>CC-CR Supermere Day 0</t>
-  </si>
-  <si>
-    <t>CC-CR Supermere Day 2</t>
-  </si>
-  <si>
-    <t>CC-CR Supermere Day 4</t>
-  </si>
-  <si>
-    <t>DiFi Exomere Day 0</t>
-  </si>
-  <si>
-    <t>DiFi Exomere Day 2</t>
-  </si>
-  <si>
-    <t>DiFi Exomere Day 4</t>
+    <t>Supermere Day 0</t>
+  </si>
+  <si>
+    <t>Supermere Day 2</t>
+  </si>
+  <si>
+    <t>Supermere Day 4</t>
   </si>
   <si>
     <t>Supermere INPUT</t>
@@ -257,36 +233,6 @@
     <t>TGFBI</t>
   </si>
   <si>
-    <t>DiFi FPLC Supermere</t>
-  </si>
-  <si>
-    <t>DiFi FPLC Exomere</t>
-  </si>
-  <si>
-    <t>DiFi UC Supermere</t>
-  </si>
-  <si>
-    <t>DiFi UC Exomere</t>
-  </si>
-  <si>
-    <t>DiFi UC sEV</t>
-  </si>
-  <si>
-    <t>CC-CR FPLC Supermere</t>
-  </si>
-  <si>
-    <t>CC-CR FPLC Exomere</t>
-  </si>
-  <si>
-    <t>CC-CR UC Supermere</t>
-  </si>
-  <si>
-    <t>CC-CR UC Exomere</t>
-  </si>
-  <si>
-    <t>CC-CR UC sEV</t>
-  </si>
-  <si>
     <t>LPS</t>
   </si>
   <si>
@@ -359,9 +305,6 @@
     <t>GE7</t>
   </si>
   <si>
-    <t>Subject</t>
-  </si>
-  <si>
     <t>Healthy 1</t>
   </si>
   <si>
@@ -465,6 +408,42 @@
   </si>
   <si>
     <t>Rna</t>
+  </si>
+  <si>
+    <t>Exomere Day 0</t>
+  </si>
+  <si>
+    <t>Exomere Day 2</t>
+  </si>
+  <si>
+    <t>Exomere Day 4</t>
+  </si>
+  <si>
+    <t>DiFi</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>CC-CR</t>
+  </si>
+  <si>
+    <t>Bakeoff</t>
+  </si>
+  <si>
+    <t>FPLC Supermere</t>
+  </si>
+  <si>
+    <t>FPLC Exomere</t>
+  </si>
+  <si>
+    <t>UC Supermere</t>
+  </si>
+  <si>
+    <t>UC Exomere</t>
+  </si>
+  <si>
+    <t>UC sEV</t>
   </si>
 </sst>
 </file>
@@ -830,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8942E758-F973-BE42-9C82-133C20AF9680}">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -847,13 +826,13 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -867,10 +846,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -884,10 +863,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -901,10 +880,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>57</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -918,10 +897,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -935,10 +914,10 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -952,15 +931,15 @@
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -969,15 +948,15 @@
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>57</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
@@ -986,15 +965,15 @@
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -1003,15 +982,15 @@
         <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -1020,15 +999,15 @@
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -1037,15 +1016,15 @@
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
@@ -1054,15 +1033,15 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -1071,15 +1050,15 @@
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -1088,15 +1067,15 @@
         <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
@@ -1105,15 +1084,15 @@
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>4</v>
@@ -1122,15 +1101,15 @@
         <v>2</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>1</v>
@@ -1139,15 +1118,15 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>4</v>
@@ -1156,15 +1135,15 @@
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>4</v>
@@ -1173,15 +1152,15 @@
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>4</v>
@@ -1190,15 +1169,15 @@
         <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -1207,15 +1186,15 @@
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>4</v>
@@ -1224,15 +1203,15 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>4</v>
@@ -1241,15 +1220,15 @@
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>4</v>
@@ -1258,10 +1237,10 @@
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1275,10 +1254,10 @@
         <v>10</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1292,10 +1271,10 @@
         <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1309,10 +1288,10 @@
         <v>10</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1326,10 +1305,10 @@
         <v>10</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>63</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1343,10 +1322,10 @@
         <v>10</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1360,15 +1339,15 @@
         <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>61</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>4</v>
@@ -1377,15 +1356,15 @@
         <v>10</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>62</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>4</v>
@@ -1394,10 +1373,10 @@
         <v>10</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>63</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1408,13 +1387,13 @@
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1425,13 +1404,13 @@
         <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1442,13 +1421,13 @@
         <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1459,13 +1438,13 @@
         <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1476,13 +1455,13 @@
         <v>4</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1493,13 +1472,13 @@
         <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1513,10 +1492,10 @@
         <v>24</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1530,10 +1509,10 @@
         <v>24</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1547,10 +1526,10 @@
         <v>24</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1564,15 +1543,15 @@
         <v>24</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>4</v>
@@ -1581,10 +1560,10 @@
         <v>24</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1595,761 +1574,761 @@
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>73</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>77</v>
+        <v>135</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>77</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>78</v>
+        <v>131</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>78</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>79</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>80</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NPX08 Heatmaps done for all experiments
</commit_message>
<xml_diff>
--- a/data/082023_Mapping_unique.xlsx
+++ b/data/082023_Mapping_unique.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olegtutanov/Documents/Programming/Olink/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A3CF91-1616-9C43-B855-03F1D1D61FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0FB380-599F-BA41-BDBA-57CEB97F1D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4480" yWindow="3180" windowWidth="25640" windowHeight="14440" xr2:uid="{2D7CE3BD-EF66-D84A-A92E-36ED3E223C28}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="139">
   <si>
     <t>SampleID</t>
   </si>
@@ -444,13 +444,22 @@
   </si>
   <si>
     <t>UC sEV</t>
+  </si>
+  <si>
+    <t>FPLC</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -465,6 +474,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -490,9 +505,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8942E758-F973-BE42-9C82-133C20AF9680}">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -818,7 +834,7 @@
     <col min="3" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -834,8 +850,11 @@
       <c r="E1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -851,8 +870,11 @@
       <c r="E2" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -868,8 +890,11 @@
       <c r="E3" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -885,8 +910,11 @@
       <c r="E4" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -902,8 +930,11 @@
       <c r="E5" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -919,8 +950,11 @@
       <c r="E6" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -936,8 +970,11 @@
       <c r="E7" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>71</v>
       </c>
@@ -953,8 +990,11 @@
       <c r="E8" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>72</v>
       </c>
@@ -970,8 +1010,11 @@
       <c r="E9" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -987,8 +1030,11 @@
       <c r="E10" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>74</v>
       </c>
@@ -1004,8 +1050,11 @@
       <c r="E11" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>75</v>
       </c>
@@ -1021,8 +1070,11 @@
       <c r="E12" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -1038,8 +1090,11 @@
       <c r="E13" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>77</v>
       </c>
@@ -1055,8 +1110,11 @@
       <c r="E14" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>78</v>
       </c>
@@ -1072,8 +1130,11 @@
       <c r="E15" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>79</v>
       </c>
@@ -1089,8 +1150,11 @@
       <c r="E16" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>80</v>
       </c>
@@ -1106,8 +1170,11 @@
       <c r="E17" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>81</v>
       </c>
@@ -1123,8 +1190,11 @@
       <c r="E18" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
@@ -1140,8 +1210,11 @@
       <c r="E19" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>83</v>
       </c>
@@ -1157,8 +1230,11 @@
       <c r="E20" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>84</v>
       </c>
@@ -1174,8 +1250,11 @@
       <c r="E21" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>85</v>
       </c>
@@ -1191,8 +1270,11 @@
       <c r="E22" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>86</v>
       </c>
@@ -1208,8 +1290,11 @@
       <c r="E23" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>87</v>
       </c>
@@ -1225,8 +1310,11 @@
       <c r="E24" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>120</v>
       </c>
@@ -1242,8 +1330,11 @@
       <c r="E25" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -1259,8 +1350,11 @@
       <c r="E26" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -1276,8 +1370,11 @@
       <c r="E27" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -1293,8 +1390,11 @@
       <c r="E28" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
@@ -1310,8 +1410,11 @@
       <c r="E29" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -1327,8 +1430,11 @@
       <c r="E30" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
@@ -1344,8 +1450,11 @@
       <c r="E31" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>88</v>
       </c>
@@ -1361,8 +1470,11 @@
       <c r="E32" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>121</v>
       </c>
@@ -1378,8 +1490,11 @@
       <c r="E33" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1395,8 +1510,11 @@
       <c r="E34" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1412,8 +1530,11 @@
       <c r="E35" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -1429,8 +1550,11 @@
       <c r="E36" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -1446,8 +1570,11 @@
       <c r="E37" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>21</v>
       </c>
@@ -1463,8 +1590,11 @@
       <c r="E38" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -1480,8 +1610,11 @@
       <c r="E39" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -1497,8 +1630,11 @@
       <c r="E40" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -1514,8 +1650,11 @@
       <c r="E41" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -1531,8 +1670,11 @@
       <c r="E42" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -1548,8 +1690,11 @@
       <c r="E43" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -1565,8 +1710,11 @@
       <c r="E44" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -1582,8 +1730,11 @@
       <c r="E45" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -1599,8 +1750,11 @@
       <c r="E46" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -1616,8 +1770,11 @@
       <c r="E47" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -1633,8 +1790,11 @@
       <c r="E48" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -1650,8 +1810,11 @@
       <c r="E49" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>33</v>
       </c>
@@ -1667,8 +1830,11 @@
       <c r="E50" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -1684,8 +1850,11 @@
       <c r="E51" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -1701,8 +1870,11 @@
       <c r="E52" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -1718,8 +1890,11 @@
       <c r="E53" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -1735,8 +1910,11 @@
       <c r="E54" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>38</v>
       </c>
@@ -1752,8 +1930,11 @@
       <c r="E55" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>39</v>
       </c>
@@ -1769,8 +1950,11 @@
       <c r="E56" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>41</v>
       </c>
@@ -1786,8 +1970,11 @@
       <c r="E57" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>42</v>
       </c>
@@ -1803,8 +1990,11 @@
       <c r="E58" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>43</v>
       </c>
@@ -1820,8 +2010,11 @@
       <c r="E59" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>44</v>
       </c>
@@ -1837,8 +2030,11 @@
       <c r="E60" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>45</v>
       </c>
@@ -1854,8 +2050,11 @@
       <c r="E61" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>96</v>
       </c>
@@ -1871,8 +2070,11 @@
       <c r="E62" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>97</v>
       </c>
@@ -1888,8 +2090,11 @@
       <c r="E63" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>98</v>
       </c>
@@ -1905,8 +2110,11 @@
       <c r="E64" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>99</v>
       </c>
@@ -1922,8 +2130,11 @@
       <c r="E65" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>100</v>
       </c>
@@ -1939,8 +2150,11 @@
       <c r="E66" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>101</v>
       </c>
@@ -1956,8 +2170,11 @@
       <c r="E67" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>102</v>
       </c>
@@ -1973,8 +2190,11 @@
       <c r="E68" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>103</v>
       </c>
@@ -1990,8 +2210,11 @@
       <c r="E69" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>104</v>
       </c>
@@ -2007,8 +2230,11 @@
       <c r="E70" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>105</v>
       </c>
@@ -2024,8 +2250,11 @@
       <c r="E71" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>106</v>
       </c>
@@ -2041,8 +2270,11 @@
       <c r="E72" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>107</v>
       </c>
@@ -2058,8 +2290,11 @@
       <c r="E73" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>108</v>
       </c>
@@ -2075,8 +2310,11 @@
       <c r="E74" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>109</v>
       </c>
@@ -2092,8 +2330,11 @@
       <c r="E75" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>110</v>
       </c>
@@ -2109,8 +2350,11 @@
       <c r="E76" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>111</v>
       </c>
@@ -2126,8 +2370,11 @@
       <c r="E77" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>112</v>
       </c>
@@ -2143,8 +2390,11 @@
       <c r="E78" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>113</v>
       </c>
@@ -2160,8 +2410,11 @@
       <c r="E79" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>114</v>
       </c>
@@ -2177,8 +2430,11 @@
       <c r="E80" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>115</v>
       </c>
@@ -2194,8 +2450,11 @@
       <c r="E81" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>116</v>
       </c>
@@ -2211,8 +2470,11 @@
       <c r="E82" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>117</v>
       </c>
@@ -2228,8 +2490,11 @@
       <c r="E83" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>118</v>
       </c>
@@ -2245,8 +2510,11 @@
       <c r="E84" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>119</v>
       </c>
@@ -2262,8 +2530,11 @@
       <c r="E85" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>122</v>
       </c>
@@ -2279,8 +2550,11 @@
       <c r="E86" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>46</v>
       </c>
@@ -2296,8 +2570,11 @@
       <c r="E87" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -2313,8 +2590,11 @@
       <c r="E88" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>49</v>
       </c>
@@ -2329,6 +2609,9 @@
       </c>
       <c r="E89" s="1" t="s">
         <v>94</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Supermere plasma vs Control+LPS heatmap
</commit_message>
<xml_diff>
--- a/data/082023_Mapping_unique.xlsx
+++ b/data/082023_Mapping_unique.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olegtutanov/Documents/Programming/Olink/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0FB380-599F-BA41-BDBA-57CEB97F1D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E566896C-483F-0B43-BA64-19064DA62C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4480" yWindow="3180" windowWidth="25640" windowHeight="14440" xr2:uid="{2D7CE3BD-EF66-D84A-A92E-36ED3E223C28}"/>
+    <workbookView xWindow="4460" yWindow="3180" windowWidth="25640" windowHeight="14440" xr2:uid="{2D7CE3BD-EF66-D84A-A92E-36ED3E223C28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
     <t>UC</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8942E758-F973-BE42-9C82-133C20AF9680}">
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F90" sqref="F90"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
NPX09 initial commit (Reformed list, dilution heatmaps)
</commit_message>
<xml_diff>
--- a/data/082023_Mapping_unique.xlsx
+++ b/data/082023_Mapping_unique.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olegtutanov/Documents/Programming/Olink/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E566896C-483F-0B43-BA64-19064DA62C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71DDA6A-23D3-1149-A487-FD7431AB00B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4460" yWindow="3180" windowWidth="25640" windowHeight="14440" xr2:uid="{2D7CE3BD-EF66-D84A-A92E-36ED3E223C28}"/>
   </bookViews>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8942E758-F973-BE42-9C82-133C20AF9680}">
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F89"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2451,7 +2451,7 @@
         <v>89</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -2471,7 +2471,7 @@
         <v>90</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -2491,7 +2491,7 @@
         <v>91</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -2511,7 +2511,7 @@
         <v>92</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -2531,7 +2531,7 @@
         <v>93</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -2551,7 +2551,7 @@
         <v>94</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>